<commit_message>
Jira Issues: PT-11, PT-15, PT-16, PT-17, PT-18, PT-19
</commit_message>
<xml_diff>
--- a/Projectboard/Projectboard/bin/Debug/requirements/Ressource Manager/template Kapazität.xlsx
+++ b/Projectboard/Projectboard/bin/Debug/requirements/Ressource Manager/template Kapazität.xlsx
@@ -11,7 +11,8 @@
     <sheet name="Kapazität" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="intern_sum">Kapazität!$A$7</definedName>
+    <definedName name="extern_sum">Kapazität!$A$11</definedName>
+    <definedName name="intern_sum">Kapazität!$A$9</definedName>
     <definedName name="Personenliste">Kapazität!$A$2:$A$6</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="24">
   <si>
     <t>Projektleiter</t>
   </si>
@@ -60,21 +61,6 @@
     <t>Innovation 1</t>
   </si>
   <si>
-    <t xml:space="preserve">Tom </t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>Friedrich</t>
-  </si>
-  <si>
-    <t>Alexander</t>
-  </si>
-  <si>
-    <t>Betty</t>
-  </si>
-  <si>
     <t>Produkt 4</t>
   </si>
   <si>
@@ -82,6 +68,30 @@
   </si>
   <si>
     <t>Angaben in PT</t>
+  </si>
+  <si>
+    <t>Summe extern</t>
+  </si>
+  <si>
+    <t>&lt;Name 1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Name 2&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Name 3&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Name 4&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Name 5&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Name Extern1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Name Extern2&gt;</t>
   </si>
 </sst>
 </file>
@@ -680,7 +690,7 @@
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="9">
@@ -876,7 +886,7 @@
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="9">
@@ -1072,7 +1082,7 @@
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="9">
@@ -1240,7 +1250,7 @@
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="5"/>
       <c r="B37" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="9">
@@ -1436,7 +1446,7 @@
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="6"/>
       <c r="B47" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="9">
@@ -1528,85 +1538,67 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A1:BL7"/>
+  <dimension ref="A1:JU11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="63" width="5.7109375" customWidth="1"/>
+    <col min="2" max="54" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:64" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:281" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B1" s="11">
-        <v>41640</v>
+        <v>41821</v>
       </c>
       <c r="C1" s="11">
-        <v>41671</v>
+        <v>41852</v>
       </c>
       <c r="D1" s="11">
-        <v>41699</v>
+        <v>41883</v>
       </c>
       <c r="E1" s="11">
-        <v>41730</v>
+        <v>41913</v>
       </c>
       <c r="F1" s="11">
-        <v>41760</v>
+        <v>41944</v>
       </c>
       <c r="G1" s="11">
-        <v>41791</v>
+        <v>41974</v>
       </c>
       <c r="H1" s="11">
-        <v>41821</v>
+        <v>42005</v>
       </c>
       <c r="I1" s="11">
-        <v>41852</v>
+        <v>42036</v>
       </c>
       <c r="J1" s="11">
-        <v>41883</v>
+        <v>42064</v>
       </c>
       <c r="K1" s="11">
-        <v>41913</v>
+        <v>42095</v>
       </c>
       <c r="L1" s="11">
-        <v>41944</v>
+        <v>42125</v>
       </c>
       <c r="M1" s="11">
-        <v>41974</v>
-      </c>
-      <c r="N1" s="11">
-        <v>42005</v>
-      </c>
-      <c r="O1" s="11">
-        <v>42036</v>
-      </c>
-      <c r="P1" s="11">
-        <v>42064</v>
-      </c>
-      <c r="Q1" s="11">
-        <v>42095</v>
-      </c>
-      <c r="R1" s="11">
-        <v>42125</v>
-      </c>
-      <c r="S1" s="11">
         <v>42156</v>
       </c>
-      <c r="T1" s="11">
-        <v>42186</v>
-      </c>
-      <c r="U1" s="11">
-        <v>42217</v>
-      </c>
-      <c r="V1" s="11">
-        <v>42248</v>
-      </c>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
       <c r="W1" s="11"/>
       <c r="X1" s="11"/>
       <c r="Y1" s="11"/>
@@ -1640,129 +1632,415 @@
       <c r="BA1" s="11"/>
       <c r="BB1" s="11"/>
       <c r="BC1" s="11"/>
-      <c r="BD1" s="11"/>
-      <c r="BE1" s="11"/>
-      <c r="BF1" s="11"/>
-      <c r="BG1" s="11"/>
-      <c r="BH1" s="11"/>
-      <c r="BI1" s="11"/>
-      <c r="BJ1" s="11"/>
-      <c r="BK1" s="11"/>
-      <c r="BL1" s="11"/>
-    </row>
-    <row r="2" spans="1:64" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:281" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:64" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:281" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:281" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:281" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:281" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:281" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:281" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:281" s="13" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B9" s="13">
+        <f t="shared" ref="B9:M9" si="0">SUM(B2:B6)</f>
+        <v>0</v>
+      </c>
+      <c r="C9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M9" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:281" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:64" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:64" s="13" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="13">
-        <f t="shared" ref="B7:V7" si="0">SUM(B2:B6)</f>
-        <v>0</v>
-      </c>
-      <c r="C7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="D7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="G7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="I7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="R7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="S7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="T7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V7" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="B11" s="13">
+        <f>SUM(B7:B8)</f>
+        <v>0</v>
+      </c>
+      <c r="C11" s="13">
+        <f t="shared" ref="C11:M11" si="1">SUM(C7:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="N11" s="13"/>
+      <c r="O11" s="13"/>
+      <c r="P11" s="13"/>
+      <c r="Q11" s="13"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="13"/>
+      <c r="AG11" s="13"/>
+      <c r="AH11" s="13"/>
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="13"/>
+      <c r="AM11" s="13"/>
+      <c r="AN11" s="13"/>
+      <c r="AO11" s="13"/>
+      <c r="AP11" s="13"/>
+      <c r="AQ11" s="13"/>
+      <c r="AR11" s="13"/>
+      <c r="AS11" s="13"/>
+      <c r="AT11" s="13"/>
+      <c r="AU11" s="13"/>
+      <c r="AV11" s="13"/>
+      <c r="AW11" s="13"/>
+      <c r="AX11" s="13"/>
+      <c r="AY11" s="13"/>
+      <c r="AZ11" s="13"/>
+      <c r="BA11" s="13"/>
+      <c r="BB11" s="13"/>
+      <c r="BC11" s="13"/>
+      <c r="BD11" s="13"/>
+      <c r="BE11" s="13"/>
+      <c r="BF11" s="13"/>
+      <c r="BG11" s="13"/>
+      <c r="BH11" s="13"/>
+      <c r="BI11" s="13"/>
+      <c r="BJ11" s="13"/>
+      <c r="BK11" s="13"/>
+      <c r="BL11" s="13"/>
+      <c r="BM11" s="13"/>
+      <c r="BN11" s="13"/>
+      <c r="BO11" s="13"/>
+      <c r="BP11" s="13"/>
+      <c r="BQ11" s="13"/>
+      <c r="BR11" s="13"/>
+      <c r="BS11" s="13"/>
+      <c r="BT11" s="13"/>
+      <c r="BU11" s="13"/>
+      <c r="BV11" s="13"/>
+      <c r="BW11" s="13"/>
+      <c r="BX11" s="13"/>
+      <c r="BY11" s="13"/>
+      <c r="BZ11" s="13"/>
+      <c r="CA11" s="13"/>
+      <c r="CB11" s="13"/>
+      <c r="CC11" s="13"/>
+      <c r="CD11" s="13"/>
+      <c r="CE11" s="13"/>
+      <c r="CF11" s="13"/>
+      <c r="CG11" s="13"/>
+      <c r="CH11" s="13"/>
+      <c r="CI11" s="13"/>
+      <c r="CJ11" s="13"/>
+      <c r="CK11" s="13"/>
+      <c r="CL11" s="13"/>
+      <c r="CM11" s="13"/>
+      <c r="CN11" s="13"/>
+      <c r="CO11" s="13"/>
+      <c r="CP11" s="13"/>
+      <c r="CQ11" s="13"/>
+      <c r="CR11" s="13"/>
+      <c r="CS11" s="13"/>
+      <c r="CT11" s="13"/>
+      <c r="CU11" s="13"/>
+      <c r="CV11" s="13"/>
+      <c r="CW11" s="13"/>
+      <c r="CX11" s="13"/>
+      <c r="CY11" s="13"/>
+      <c r="CZ11" s="13"/>
+      <c r="DA11" s="13"/>
+      <c r="DB11" s="13"/>
+      <c r="DC11" s="13"/>
+      <c r="DD11" s="13"/>
+      <c r="DE11" s="13"/>
+      <c r="DF11" s="13"/>
+      <c r="DG11" s="13"/>
+      <c r="DH11" s="13"/>
+      <c r="DI11" s="13"/>
+      <c r="DJ11" s="13"/>
+      <c r="DK11" s="13"/>
+      <c r="DL11" s="13"/>
+      <c r="DM11" s="13"/>
+      <c r="DN11" s="13"/>
+      <c r="DO11" s="13"/>
+      <c r="DP11" s="13"/>
+      <c r="DQ11" s="13"/>
+      <c r="DR11" s="13"/>
+      <c r="DS11" s="13"/>
+      <c r="DT11" s="13"/>
+      <c r="DU11" s="13"/>
+      <c r="DV11" s="13"/>
+      <c r="DW11" s="13"/>
+      <c r="DX11" s="13"/>
+      <c r="DY11" s="13"/>
+      <c r="DZ11" s="13"/>
+      <c r="EA11" s="13"/>
+      <c r="EB11" s="13"/>
+      <c r="EC11" s="13"/>
+      <c r="ED11" s="13"/>
+      <c r="EE11" s="13"/>
+      <c r="EF11" s="13"/>
+      <c r="EG11" s="13"/>
+      <c r="EH11" s="13"/>
+      <c r="EI11" s="13"/>
+      <c r="EJ11" s="13"/>
+      <c r="EK11" s="13"/>
+      <c r="EL11" s="13"/>
+      <c r="EM11" s="13"/>
+      <c r="EN11" s="13"/>
+      <c r="EO11" s="13"/>
+      <c r="EP11" s="13"/>
+      <c r="EQ11" s="13"/>
+      <c r="ER11" s="13"/>
+      <c r="ES11" s="13"/>
+      <c r="ET11" s="13"/>
+      <c r="EU11" s="13"/>
+      <c r="EV11" s="13"/>
+      <c r="EW11" s="13"/>
+      <c r="EX11" s="13"/>
+      <c r="EY11" s="13"/>
+      <c r="EZ11" s="13"/>
+      <c r="FA11" s="13"/>
+      <c r="FB11" s="13"/>
+      <c r="FC11" s="13"/>
+      <c r="FD11" s="13"/>
+      <c r="FE11" s="13"/>
+      <c r="FF11" s="13"/>
+      <c r="FG11" s="13"/>
+      <c r="FH11" s="13"/>
+      <c r="FI11" s="13"/>
+      <c r="FJ11" s="13"/>
+      <c r="FK11" s="13"/>
+      <c r="FL11" s="13"/>
+      <c r="FM11" s="13"/>
+      <c r="FN11" s="13"/>
+      <c r="FO11" s="13"/>
+      <c r="FP11" s="13"/>
+      <c r="FQ11" s="13"/>
+      <c r="FR11" s="13"/>
+      <c r="FS11" s="13"/>
+      <c r="FT11" s="13"/>
+      <c r="FU11" s="13"/>
+      <c r="FV11" s="13"/>
+      <c r="FW11" s="13"/>
+      <c r="FX11" s="13"/>
+      <c r="FY11" s="13"/>
+      <c r="FZ11" s="13"/>
+      <c r="GA11" s="13"/>
+      <c r="GB11" s="13"/>
+      <c r="GC11" s="13"/>
+      <c r="GD11" s="13"/>
+      <c r="GE11" s="13"/>
+      <c r="GF11" s="13"/>
+      <c r="GG11" s="13"/>
+      <c r="GH11" s="13"/>
+      <c r="GI11" s="13"/>
+      <c r="GJ11" s="13"/>
+      <c r="GK11" s="13"/>
+      <c r="GL11" s="13"/>
+      <c r="GM11" s="13"/>
+      <c r="GN11" s="13"/>
+      <c r="GO11" s="13"/>
+      <c r="GP11" s="13"/>
+      <c r="GQ11" s="13"/>
+      <c r="GR11" s="13"/>
+      <c r="GS11" s="13"/>
+      <c r="GT11" s="13"/>
+      <c r="GU11" s="13"/>
+      <c r="GV11" s="13"/>
+      <c r="GW11" s="13"/>
+      <c r="GX11" s="13"/>
+      <c r="GY11" s="13"/>
+      <c r="GZ11" s="13"/>
+      <c r="HA11" s="13"/>
+      <c r="HB11" s="13"/>
+      <c r="HC11" s="13"/>
+      <c r="HD11" s="13"/>
+      <c r="HE11" s="13"/>
+      <c r="HF11" s="13"/>
+      <c r="HG11" s="13"/>
+      <c r="HH11" s="13"/>
+      <c r="HI11" s="13"/>
+      <c r="HJ11" s="13"/>
+      <c r="HK11" s="13"/>
+      <c r="HL11" s="13"/>
+      <c r="HM11" s="13"/>
+      <c r="HN11" s="13"/>
+      <c r="HO11" s="13"/>
+      <c r="HP11" s="13"/>
+      <c r="HQ11" s="13"/>
+      <c r="HR11" s="13"/>
+      <c r="HS11" s="13"/>
+      <c r="HT11" s="13"/>
+      <c r="HU11" s="13"/>
+      <c r="HV11" s="13"/>
+      <c r="HW11" s="13"/>
+      <c r="HX11" s="13"/>
+      <c r="HY11" s="13"/>
+      <c r="HZ11" s="13"/>
+      <c r="IA11" s="13"/>
+      <c r="IB11" s="13"/>
+      <c r="IC11" s="13"/>
+      <c r="ID11" s="13"/>
+      <c r="IE11" s="13"/>
+      <c r="IF11" s="13"/>
+      <c r="IG11" s="13"/>
+      <c r="IH11" s="13"/>
+      <c r="II11" s="13"/>
+      <c r="IJ11" s="13"/>
+      <c r="IK11" s="13"/>
+      <c r="IL11" s="13"/>
+      <c r="IM11" s="13"/>
+      <c r="IN11" s="13"/>
+      <c r="IO11" s="13"/>
+      <c r="IP11" s="13"/>
+      <c r="IQ11" s="13"/>
+      <c r="IR11" s="13"/>
+      <c r="IS11" s="13"/>
+      <c r="IT11" s="13"/>
+      <c r="IU11" s="13"/>
+      <c r="IV11" s="13"/>
+      <c r="IW11" s="13"/>
+      <c r="IX11" s="13"/>
+      <c r="IY11" s="13"/>
+      <c r="IZ11" s="13"/>
+      <c r="JA11" s="13"/>
+      <c r="JB11" s="13"/>
+      <c r="JC11" s="13"/>
+      <c r="JD11" s="13"/>
+      <c r="JE11" s="13"/>
+      <c r="JF11" s="13"/>
+      <c r="JG11" s="13"/>
+      <c r="JH11" s="13"/>
+      <c r="JI11" s="13"/>
+      <c r="JJ11" s="13"/>
+      <c r="JK11" s="13"/>
+      <c r="JL11" s="13"/>
+      <c r="JM11" s="13"/>
+      <c r="JN11" s="13"/>
+      <c r="JO11" s="13"/>
+      <c r="JP11" s="13"/>
+      <c r="JQ11" s="13"/>
+      <c r="JR11" s="13"/>
+      <c r="JS11" s="13"/>
+      <c r="JT11" s="13"/>
+      <c r="JU11" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>